<commit_message>
Avance 1 - Tesis 1
</commit_message>
<xml_diff>
--- a/Avance 1.xlsx
+++ b/Avance 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abraham\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abraham\Desktop\UPN\TesisAgricola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28054A69-66A6-40D2-B16D-17A3EA2C0E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952E25A1-DAFC-47A7-B9B6-E4E5FF84DA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BDED7A33-3EBB-4B0F-A96B-1A4678AA2FE0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>propuesta fundamentada en problema que amerita una investigación</t>
   </si>
@@ -56,15 +56,6 @@
     <t>Contexto:</t>
   </si>
   <si>
-    <t>Elementos de la pregunta de investigación</t>
-  </si>
-  <si>
-    <t>Enunciado interrogativo (Pregunta de investigación)</t>
-  </si>
-  <si>
-    <t>TITULO TENTATIVO DE LA REVISIÓN SISTEMÁTICA</t>
-  </si>
-  <si>
     <t>RESUMEN</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
     <t>Descriptiva propositiva</t>
   </si>
   <si>
-    <t>Agricultores nacionales afectados por los fenomenos climatológicos</t>
-  </si>
-  <si>
     <t>Perdida de cultivos y su calidad</t>
   </si>
   <si>
@@ -117,6 +105,36 @@
   </si>
   <si>
     <t>Título</t>
+  </si>
+  <si>
+    <t>Cultivo tradicional</t>
+  </si>
+  <si>
+    <t>Seguridad de la obtención del producto final</t>
+  </si>
+  <si>
+    <t>Condiciones adversas para el cultivo</t>
+  </si>
+  <si>
+    <t>Tema Especifico</t>
+  </si>
+  <si>
+    <t>Enunciado interrogativo</t>
+  </si>
+  <si>
+    <t>Elementos del enunciado del estudio</t>
+  </si>
+  <si>
+    <t>¿Cuál es el impacto de los fenómenos climatológicos en los campos de cultivo y como afectan a los agricultores en la región norte del Perú en los últimos 3 años?</t>
+  </si>
+  <si>
+    <t>Agricultores nacionales en zonas rurales afectados por los fenómenos climatológicos</t>
+  </si>
+  <si>
+    <t>Metodología de un sistema de protección de cultivo</t>
+  </si>
+  <si>
+    <t>En el Perú se presentan fenómenos climáticos como "el niño costero" y "la niña", sin embargo en este año 2023 se ha presentado un ciclón llamado “Yaku” que ha impactado a varios sectores del país, entre ellos tenemos al sector agrícola, que ha sido afectado por pérdidas de cultivos, erosión del suelo, entre otros; por ello el presente proyecto se enfoca en una metodología que apoye al desarrollo de un sistema con fines de lograr la protección de los cultivos minimizando los impactos negativos y apoyar a este sector con la seguridad de obtención del cultivo de buena calidad.</t>
   </si>
 </sst>
 </file>
@@ -170,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,8 +201,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -192,25 +240,163 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -227,6 +413,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>384643</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>106018</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>776195</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>117190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A453BB0-6111-1BE6-52D5-8204B8E7F1BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8110660" y="1775792"/>
+          <a:ext cx="8342857" cy="3390476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -526,191 +761,233 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E737C38-B6A2-4871-BE8B-1F0429EB453B}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="46.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J2" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F3" t="s">
+      <c r="C2" t="s">
         <v>0</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4"/>
+      <c r="B13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A12:A29"/>
+  <mergeCells count="7">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B21:D26"/>
+    <mergeCell ref="A12:A26"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="A4:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>